<commit_message>
allow keys in permitted operations
</commit_message>
<xml_diff>
--- a/binary_storage/submission.xlsx
+++ b/binary_storage/submission.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
   <si>
     <t>x</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>exp</t>
+  </si>
+  <si>
+    <t>Not Implemented</t>
   </si>
   <si>
     <t>(0.00016895996361733495-0.00028569569600170796j)</t>
@@ -497,8 +500,8 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
-        <v>14.79</v>
+      <c r="D5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -554,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -694,7 +697,7 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -791,8 +794,8 @@
       <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="D26">
-        <v>1.628919860627178</v>
+      <c r="D26" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -945,8 +948,8 @@
       <c r="C37" t="s">
         <v>11</v>
       </c>
-      <c r="D37">
-        <v>4.42</v>
+      <c r="D37" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -974,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1002,7 +1005,7 @@
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1044,7 +1047,7 @@
         <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1113,8 +1116,8 @@
       <c r="C49" t="s">
         <v>12</v>
       </c>
-      <c r="D49">
-        <v>13.49224648004349</v>
+      <c r="D49" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:4">

</xml_diff>

<commit_message>
results rounded to 2 decimal place, util function added
</commit_message>
<xml_diff>
--- a/binary_storage/submission.xlsx
+++ b/binary_storage/submission.xlsx
@@ -58,19 +58,19 @@
     <t>Not Implemented</t>
   </si>
   <si>
-    <t>(0.00016895996361733495-0.00028569569600170796j)</t>
-  </si>
-  <si>
-    <t>(4509860.2935963+35699220.158200406j)</t>
-  </si>
-  <si>
-    <t>(3250.5479008637303-2689.087087424294j)</t>
+    <t>0j</t>
+  </si>
+  <si>
+    <t>(4509860.29+35699220.16j)</t>
+  </si>
+  <si>
+    <t>(3250.55-2689.09j)</t>
   </si>
   <si>
     <t>Not Divisible</t>
   </si>
   <si>
-    <t>(-9399580760441.664-19975125898265.56j)</t>
+    <t>(-9399580760441.66-19975125898265.56j)</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>7.240000000000002</v>
+        <v>7.24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -473,7 +473,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>14.0384</v>
+        <v>14.04</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -487,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>3.035732662007217</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -515,7 +515,7 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>-3.091787439613527</v>
+        <v>-3.09</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="D7">
-        <v>-0.9200000000000002</v>
+        <v>-0.92</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -543,7 +543,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>-7.476000000000001</v>
+        <v>-7.48</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -613,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="D13">
-        <v>-1.3395</v>
+        <v>-1.34</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -627,7 +627,7 @@
         <v>6</v>
       </c>
       <c r="D14">
-        <v>83.92325948513293</v>
+        <v>83.92</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -655,7 +655,7 @@
         <v>8</v>
       </c>
       <c r="D16">
-        <v>-1.319311663479924</v>
+        <v>-1.32</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -711,7 +711,7 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>1.959999999999999</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -725,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="D21">
-        <v>-0.9396984924623116</v>
+        <v>-0.9399999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -753,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="D23">
-        <v>68.9186</v>
+        <v>68.92</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -767,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="D24">
-        <v>6.562074640300713E-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="D28">
-        <v>4.6788</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -837,7 +837,7 @@
         <v>6</v>
       </c>
       <c r="D29">
-        <v>0.004498660346273822</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -865,7 +865,7 @@
         <v>8</v>
       </c>
       <c r="D31">
-        <v>-0.1894904458598726</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -893,7 +893,7 @@
         <v>5</v>
       </c>
       <c r="D33">
-        <v>5.1496</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -907,7 +907,7 @@
         <v>6</v>
       </c>
       <c r="D34">
-        <v>5167627653018.042</v>
+        <v>5167627653018.04</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -935,7 +935,7 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <v>-2.118421052631579</v>
+        <v>-2.12</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -963,7 +963,7 @@
         <v>5</v>
       </c>
       <c r="D38">
-        <v>-98.193</v>
+        <v>-98.19</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1075,7 +1075,7 @@
         <v>8</v>
       </c>
       <c r="D46">
-        <v>-0.008326394671107412</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1103,7 +1103,7 @@
         <v>5</v>
       </c>
       <c r="D48">
-        <v>180.7701</v>
+        <v>180.77</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1145,7 +1145,7 @@
         <v>8</v>
       </c>
       <c r="D51">
-        <v>-10.77551020408163</v>
+        <v>-10.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>